<commit_message>
working on intent pattern
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\chatbot demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\chatbot-demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11832"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11832" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t>Questions</t>
   </si>
@@ -176,6 +177,19 @@
 I want to know more about Future-Proofed Contact Center
 What is Future-Proofed Contact Center?
 </t>
+  </si>
+  <si>
+    <t>Free package ($0/Month) offers:
+1. Automated Routing 
+2.Interactive Voice Response &lt;br/&gt;&lt;br/&gt; 3. Chatbots &lt;br/&gt;&lt;br/&gt; 4. Analytics and Reporting</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Mega Cloud&lt;/strong&gt; provides personalized, omnichannel customer support from a single interface through our cloud-based contact center solution. Some of the attractive features of Mega Cloud are:
+1. Omnichannel Management
+2. Future-Proofed Contact Center
+3.Chatbots with Text-to-Speech Capabilties
+4.Workforce Management Integration
+5.Built-In AI Routing Two-Way Messaging</t>
   </si>
 </sst>
 </file>
@@ -547,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,4 +727,176 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="47.44140625" customWidth="1"/>
+    <col min="2" max="2" width="72.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel & pattern changes
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>Questions</t>
   </si>
@@ -179,24 +179,93 @@
 </t>
   </si>
   <si>
+    <t>A few of many agent deskop features are: 
+1. See the full picture with contextual details about customer history and preferences
+2.  Manage all conversations in one streamlined interface. Field inbound messages or place outbound calls using a personalized directory
+3. View and track individual agent performance metrics like AHT, FCR, and more</t>
+  </si>
+  <si>
     <t>Free package ($0/Month) offers:
 1. Automated Routing 
-2.Interactive Voice Response &lt;br/&gt;&lt;br/&gt; 3. Chatbots &lt;br/&gt;&lt;br/&gt; 4. Analytics and Reporting</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;Mega Cloud&lt;/strong&gt; provides personalized, omnichannel customer support from a single interface through our cloud-based contact center solution. Some of the attractive features of Mega Cloud are:
+2.Interactive Voice Response
+3. Chatbots
+4. Analytics and Reporting</t>
+  </si>
+  <si>
+    <t>Mega Cloud is available in three flavors at a variety of affordable price points. 
+1. Free - $0/mo
+2. Premium - $99/mo
+3. Platinum - $170/mo</t>
+  </si>
+  <si>
+    <t>Premium package ($99/Month) offers:
+1. Automated Routing
+2.Interactive Voice Response 
+3. Chatbots
+4. Analytics and Reporting
+5. Third Party Integration</t>
+  </si>
+  <si>
+    <t>Platinum package ($170/Month) offers:
+1. Automated Routing
+2.Interactive Voice Response
+3. Chatbots 
+4. Analytics and Reporting
+5. Third Party Integration</t>
+  </si>
+  <si>
+    <t>Free package ($0/Month) offers:
+1. Automated Routing
+2.Interactive Voice Response
+3. Chatbots
+4. Analytics and Reporting 
+Premium package ($99/Month) offers: 
+1. Automated Routing 
+2.Interactive Voice Response
+3. Chatbots
+4. Analytics and Reporting
+5. Third Party Integration
+Platinum package ($170/Month) offers: 
+1. Automated Routing 
+2. Interactive Voice Response 
+3. Chatbots
+4. Analytics and Reporting
+5. Third Party Integration</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mega Cloud</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  provides personalized, omnichannel customer support from a single interface through our cloud-based contact center solution. Some of the attractive features of Mega Cloud are:
 1. Omnichannel Management
 2. Future-Proofed Contact Center
 3.Chatbots with Text-to-Speech Capabilties
 4.Workforce Management Integration
 5.Built-In AI Routing Two-Way Messaging</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +276,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -733,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,7 +833,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -812,47 +889,47 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>